<commit_message>
Minor style change in users.xlsx
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/users.xlsx
+++ b/MewPipe.DataFeeder/datas/users.xlsx
@@ -42,7 +42,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +60,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,7 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -405,7 +413,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
You had one job ! -_-
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/users.xlsx
+++ b/MewPipe.DataFeeder/datas/users.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>User</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Légère préférence pour une catégorie avec peu de like au total</t>
+  </si>
+  <si>
+    <t>Govinda Dimosthenis</t>
+  </si>
+  <si>
+    <t>Azarel Feodosiy</t>
+  </si>
+  <si>
+    <t>Jarah Aaron</t>
+  </si>
+  <si>
+    <t>Peder Oddmund</t>
+  </si>
+  <si>
+    <t>Ashok Walganus</t>
+  </si>
+  <si>
+    <t>Royle Faust</t>
+  </si>
+  <si>
+    <t>Azhar Drake</t>
+  </si>
+  <si>
+    <t>Artur Emil</t>
+  </si>
+  <si>
+    <t>Yoshirou Harvie</t>
   </si>
 </sst>
 </file>
@@ -137,18 +164,18 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
@@ -434,7 +461,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,19 +473,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
@@ -467,7 +494,9 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="B2">
         <v>80</v>
       </c>
@@ -482,7 +511,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="B3">
         <v>10</v>
       </c>
@@ -495,7 +526,9 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="B4">
         <v>10</v>
       </c>
@@ -508,7 +541,9 @@
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="B5">
         <v>50</v>
       </c>
@@ -523,14 +558,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
         <v>70</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>70</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -538,7 +575,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="B7">
         <v>10</v>
       </c>
@@ -551,14 +590,16 @@
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
         <v>90</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>60</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -566,7 +607,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="B9">
         <v>60</v>
       </c>
@@ -579,31 +622,33 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
         <v>30</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>20</v>
       </c>
-      <c r="D10" s="3">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fixed recommendations score & User likes
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/users.xlsx
+++ b/MewPipe.DataFeeder/datas/users.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>User</t>
   </si>
@@ -31,24 +31,6 @@
   </si>
   <si>
     <t>Music (%)</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Les 3 premiers users ont une préférence nette pour une catégorie</t>
-  </si>
-  <si>
-    <t>Si un user like toutes les catégories de manière égale, on pourrait mieux voir l'effet des dislikes dans la suggestion</t>
-  </si>
-  <si>
-    <t>Préférence pour 2 catégories de manière égale</t>
-  </si>
-  <si>
-    <t>Préférence pour 2 catégories de manière inégale</t>
-  </si>
-  <si>
-    <t>Légère préférence pour une catégorie avec peu de like au total</t>
   </si>
   <si>
     <t>Govinda Dimosthenis</t>
@@ -161,10 +143,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -172,10 +153,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
@@ -461,7 +442,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,182 +454,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>80</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2">
-        <v>70</v>
-      </c>
-      <c r="D6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>70</v>
-      </c>
-      <c r="D7">
-        <v>70</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3">
-        <v>90</v>
-      </c>
-      <c r="C8" s="3">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3">
-        <v>10</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>60</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>90</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>10</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added more users for impressions (27 users)
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/users.xlsx
+++ b/MewPipe.DataFeeder/datas/users.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>User</t>
   </si>
@@ -58,6 +58,60 @@
   </si>
   <si>
     <t>Yoshirou Harvie</t>
+  </si>
+  <si>
+    <t>Teodors Kekoa</t>
+  </si>
+  <si>
+    <t>Ophir Florent</t>
+  </si>
+  <si>
+    <t>Cleon Beso</t>
+  </si>
+  <si>
+    <t>Corentin Samoil</t>
+  </si>
+  <si>
+    <t>Sorley Itamar</t>
+  </si>
+  <si>
+    <t>Nelom Fletcher</t>
+  </si>
+  <si>
+    <t>Peter Seth</t>
+  </si>
+  <si>
+    <t>Stan Stjepan</t>
+  </si>
+  <si>
+    <t>Quintin Ervin</t>
+  </si>
+  <si>
+    <t>Ajith Jozo</t>
+  </si>
+  <si>
+    <t>Plutarch Sam</t>
+  </si>
+  <si>
+    <t>Emem Jodoc</t>
+  </si>
+  <si>
+    <t>Fedlimid Robert</t>
+  </si>
+  <si>
+    <t>Headley Jaume</t>
+  </si>
+  <si>
+    <t>Sophus Makana</t>
+  </si>
+  <si>
+    <t>Enok Ognian</t>
+  </si>
+  <si>
+    <t>Nico Felinus</t>
+  </si>
+  <si>
+    <t>Neptune Leonardo</t>
   </si>
 </sst>
 </file>
@@ -439,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,10 +546,10 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -507,13 +561,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -522,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -536,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -551,13 +605,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -566,7 +620,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -581,10 +635,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -596,27 +650,269 @@
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
       </c>
       <c r="D10" s="2">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>80</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>100</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D28" s="2">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>